<commit_message>
change target execution kpis
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2019/KPIConversion2019.xlsx
+++ b/Projects/CCRU/Data/KPIs_2019/KPIConversion2019.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -154,10 +154,7 @@
     <t xml:space="preserve">Any Other Activation</t>
   </si>
   <si>
-    <t xml:space="preserve">Adez Warm Shelf Share</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adez Cold Shelf Share</t>
+    <t xml:space="preserve">Adez Shelf Share</t>
   </si>
 </sst>
 </file>
@@ -356,17 +353,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.9591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.5510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.4234693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -719,14 +715,6 @@
       </c>
       <c r="B44" s="4" t="n">
         <v>43</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B45" s="4" t="n">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>